<commit_message>
feat: added api for applicants database
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BB09B-0F57-4E93-A3AE-9E4DA26ACE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACBE29-5BF3-4FD5-A4A9-E0E6581DF355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="10635" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="15690" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1516,13 +1516,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: login api and applicant info reducer
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACBE29-5BF3-4FD5-A4A9-E0E6581DF355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942EC16A-1F97-44BD-BDBF-ACF0BDE16154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15" windowWidth="15690" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,8 +1006,8 @@
   </sheetPr>
   <dimension ref="B1:BO31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: profile picture upload and addition to appointment modal
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942EC16A-1F97-44BD-BDBF-ACF0BDE16154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C3F798-5A57-450F-860A-69FF9BCD680C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="15690" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: added api for applications collection
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C3F798-5A57-450F-860A-69FF9BCD680C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA97F2B7-80DF-4AA9-8101-DD1220568E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1519,10 +1519,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="8">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: updated application details
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF34F1-425E-4A3B-B09A-0E191D5063C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C6D92-D99E-449A-BDFB-A55BD50950D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15:R15"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1519,10 +1519,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" s="8">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: added backend for uploading documents
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904C6D92-D99E-449A-BDFB-A55BD50950D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE84CE4E-4017-46F8-9DB0-2FF681EF7AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1522,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="8">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: added upload receipt
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE84CE4E-4017-46F8-9DB0-2FF681EF7AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D42DA-32E0-45EE-BB04-67BEE2C0A917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AF14" sqref="AF14"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1519,10 +1519,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="8">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: added appointment date setter and change avatar button
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D42DA-32E0-45EE-BB04-67BEE2C0A917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800E47B-6228-4B35-ADAA-0D2193A612B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
       <c r="G12" s="8">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1536,10 +1536,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
feat: css for login and registration page
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0800E47B-6228-4B35-ADAA-0D2193A612B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E635BC-4257-4EA4-ABFD-303B206E1881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1556,13 +1556,13 @@
         <v>2</v>
       </c>
       <c r="E14" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: main page ang profile tab css
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E635BC-4257-4EA4-ABFD-303B206E1881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78494EE2-B069-4EC7-9CD1-318E9E137D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1559,10 +1559,10 @@
         <v>10</v>
       </c>
       <c r="F14" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="8">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: appointment tab css
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78494EE2-B069-4EC7-9CD1-318E9E137D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B402A1-050C-49A6-B948-3D11FF3ED0D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>PERIODS</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Create interface and backend for reviewer</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1559,19 +1562,21 @@
         <v>10</v>
       </c>
       <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7">
+        <v>12</v>
+      </c>
+      <c r="D15" s="7">
         <v>3</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
feat: updated redux related code and more css
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B402A1-050C-49A6-B948-3D11FF3ED0D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E69748-9C40-4A26-A98D-069053900B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1579,13 +1579,13 @@
         <v>3</v>
       </c>
       <c r="E15" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: reviewer interface - 50%
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E69748-9C40-4A26-A98D-069053900B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583AAC06-F658-4C67-A1F2-7FBA026D5502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1585,7 +1585,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="8">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: local storage and reviewer interface
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583AAC06-F658-4C67-A1F2-7FBA026D5502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6928636B-3BF5-4BC1-BF72-0E441CE951E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1585,7 +1585,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="8">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: set appointment date filter
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6928636B-3BF5-4BC1-BF72-0E441CE951E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1286C85C-3196-4FFD-A66C-B39B025AA6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1539,13 +1539,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1582,10 +1582,10 @@
         <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="8">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: reviewer logout button and bugfixes
</commit_message>
<xml_diff>
--- a/other files/Project Plan.xlsx
+++ b/other files/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Github\online-appointment-system\other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1286C85C-3196-4FFD-A66C-B39B025AA6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA923E-1172-410E-8372-C8C5BB20126E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1582,7 +1582,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>

</xml_diff>